<commit_message>
Turn off economic retirements for hydro.
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FDBFBA6-B529-49A7-A4EF-4EC1C6ADD991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC0C12-BC57-4F02-8B26-0EBFF568F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>CRpUNL Capacity Retired per Unit Net Loss</t>
+  </si>
+  <si>
+    <t>Hydro plants typically have other revenue streams and other considerations when determining whether or not to retire them,</t>
+  </si>
+  <si>
+    <t>so we assume a value of zero</t>
   </si>
 </sst>
 </file>
@@ -171,12 +177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -191,13 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +564,16 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +589,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,8 +641,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>159.27199999999999</v>
+      <c r="B6" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +721,7 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -706,7 +729,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>0</v>
       </c>
     </row>
@@ -722,7 +745,7 @@
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -730,7 +753,7 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -738,7 +761,7 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>0</v>
       </c>
     </row>
@@ -746,7 +769,7 @@
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>0</v>
       </c>
     </row>
@@ -754,7 +777,7 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>0</v>
       </c>
     </row>
@@ -762,7 +785,7 @@
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>0</v>
       </c>
     </row>
@@ -770,7 +793,7 @@
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates for 4.0.1. Address a bug with calculating marginal disptach costs by hour, updates retirement mechanism and data to work in terms of MW/($/MW), address hydro data issues; updates economic retirement parameters for coal and updates BAU retirements to align with 111 rules.
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CRpUNL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC0C12-BC57-4F02-8B26-0EBFF568F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A2D67-3F06-44C3-AAA2-D5E31B535A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="30" yWindow="15" windowWidth="23010" windowHeight="13770" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -96,9 +96,6 @@
     <t>municipal solid waste</t>
   </si>
   <si>
-    <t>Fraction of start year capacity</t>
-  </si>
-  <si>
     <t>hard coal w CCS</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Certain plant types are less prone to economic retirement because they are maintained for local reliability purposes.</t>
   </si>
   <si>
-    <t xml:space="preserve">These includes: natural gas steam turbines, natural gas peakers, and petroleum plants. For these plant types we set the </t>
-  </si>
-  <si>
     <t>retirement fraction very low.</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>hydrogen combined cycle</t>
   </si>
   <si>
-    <t>Unit: MW/($/MWh)</t>
-  </si>
-  <si>
     <t>CRpUNL Capacity Retired per Unit Net Loss</t>
   </si>
   <si>
@@ -139,6 +130,21 @@
   </si>
   <si>
     <t>so we assume a value of zero</t>
+  </si>
+  <si>
+    <t>MW retired</t>
+  </si>
+  <si>
+    <t>Unit: MW/($/MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These includes: natural gas steam turbines and petroleum plants. For these plant types we set the </t>
+  </si>
+  <si>
+    <t>Likewise, biomass plants are often colocated with cheap supply and part of integrated</t>
+  </si>
+  <si>
+    <t>CHP or industrial systems, and we therefore do not subject them to economic retirement.</t>
   </si>
 </sst>
 </file>
@@ -525,17 +531,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,27 +559,37 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +605,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,10 +615,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -610,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>422.61599999999999</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -618,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7.2404799999999998</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>536.64700000000005</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>193.001</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>236.00399999999999</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -658,39 +674,39 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>91.676199999999994</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>3.4958</v>
+      <c r="B9" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>21.655999999999999</v>
+      <c r="B10" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>5.0449999999999999</v>
+      <c r="B11" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>2.41744</v>
+      <c r="B12" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>12.7104</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +722,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>5.2843999999999998</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>5.8599999999999999E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,64 +753,64 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <v>3.5217999999999998</v>
+      <c r="B18" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset coal retirements data to align with EPA 111 RIA
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCD4A74-57F3-42DA-9B20-0FA833A3D045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C4A85-6A1E-41E5-8FBD-A2A66D513898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Recalibrate retirements per unit net loss parameter
</commit_message>
<xml_diff>
--- a/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
+++ b/InputData/elec/CRpUNL/Cap Ret per Unit Net Loss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CRpUNL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us-analysis\InputData\elec\CRpUNL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C4A85-6A1E-41E5-8FBD-A2A66D513898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6567EA64-6F7D-43AE-A26B-B09A74E72F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -183,18 +183,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,14 +203,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -604,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +627,8 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +636,8 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,14 +645,15 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
@@ -666,7 +662,8 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,14 +671,15 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
@@ -689,7 +687,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
@@ -697,7 +695,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
@@ -705,7 +703,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>0</v>
       </c>
     </row>
@@ -714,7 +712,8 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +721,8 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,14 +730,15 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.03</v>
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>0</v>
       </c>
     </row>
@@ -745,7 +746,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>0</v>
       </c>
     </row>
@@ -753,7 +754,7 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>0</v>
       </c>
     </row>
@@ -761,56 +762,63 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.03</v>
+      <c r="B19">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4">
-        <v>0.03</v>
+      <c r="B20">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4">
-        <v>0.03</v>
+      <c r="B21">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.03</v>
+      <c r="B22">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4">
-        <v>0.03</v>
+      <c r="B23">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4">
-        <v>0.03</v>
+      <c r="B24">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4">
-        <v>0.03</v>
+      <c r="B25">
+        <f>$B$2</f>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>